<commit_message>
updated seed collection list with hickory
</commit_message>
<xml_diff>
--- a/data/Seed_collection.xlsx
+++ b/data/Seed_collection.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/catchamberlain/Documents/git/freezingexperiment/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/CatherineChamberlain/Documents/git/freezingexperiment/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="29980" yWindow="460" windowWidth="28800" windowHeight="17600" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="meta" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="76">
   <si>
     <t>Experiment Work:</t>
   </si>
@@ -253,6 +253,9 @@
   </si>
   <si>
     <t>northern north america</t>
+  </si>
+  <si>
+    <t>CAROVA</t>
   </si>
 </sst>
 </file>
@@ -668,10 +671,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1090,6 +1093,29 @@
         <v>49</v>
       </c>
     </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>75</v>
+      </c>
+      <c r="B19" t="s">
+        <v>60</v>
+      </c>
+      <c r="C19" t="s">
+        <v>26</v>
+      </c>
+      <c r="D19" t="s">
+        <v>27</v>
+      </c>
+      <c r="E19" t="s">
+        <v>36</v>
+      </c>
+      <c r="F19" t="s">
+        <v>29</v>
+      </c>
+      <c r="G19" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>